<commit_message>
Update data before the retrospective
</commit_message>
<xml_diff>
--- a/feebacks-timesheets/Sprint8_Timesheet.xlsx
+++ b/feebacks-timesheets/Sprint8_Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asarpa\Desktop\thesis\feebacks-timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1287C176-4DCA-4A85-B334-4AEA8246E04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F09C60-F08B-4414-B521-888DF2C9331E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
   <si>
     <t>Amedeo</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Add the number of selcted consulants</t>
   </si>
   <si>
-    <t>Approve/deny request from notifications</t>
-  </si>
-  <si>
     <t>add statistics about consultant</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
   </si>
   <si>
     <t>tenant implementation</t>
-  </si>
-  <si>
-    <t>sort lists</t>
   </si>
   <si>
     <t>Create a consultant</t>
@@ -602,28 +596,28 @@
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:M20"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.140625" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="1" max="1" width="41.109375" customWidth="1"/>
+    <col min="2" max="2" width="42.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" customWidth="1"/>
     <col min="6" max="6" width="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
-    <col min="11" max="11" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" customWidth="1"/>
+    <col min="11" max="11" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>20</v>
       </c>
@@ -640,7 +634,7 @@
       <c r="L1" s="18"/>
       <c r="M1" s="18"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18"/>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -655,7 +649,7 @@
       <c r="L2" s="18"/>
       <c r="M2" s="18"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -670,7 +664,7 @@
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
     </row>
-    <row r="4" spans="1:15" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11"/>
       <c r="B4" s="12" t="s">
         <v>22</v>
@@ -681,37 +675,33 @@
       <c r="D4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="H4" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="J4" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="15" t="s">
+      <c r="K4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="15" t="s">
+      <c r="L4" s="12"/>
+      <c r="M4" s="12" t="s">
         <v>31</v>
-      </c>
-      <c r="L4" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="M4" s="12" t="s">
-        <v>33</v>
       </c>
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
     </row>
-    <row r="5" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>0</v>
       </c>
@@ -724,9 +714,7 @@
       <c r="D5" s="13">
         <v>0</v>
       </c>
-      <c r="E5" s="13">
-        <v>0</v>
-      </c>
+      <c r="E5" s="13"/>
       <c r="F5" s="13">
         <v>0</v>
       </c>
@@ -740,21 +728,19 @@
         <v>0</v>
       </c>
       <c r="J5" s="13">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K5" s="13">
-        <v>12</v>
-      </c>
-      <c r="L5" s="13">
-        <v>0</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="L5" s="13"/>
       <c r="M5" s="13">
         <v>0</v>
       </c>
       <c r="N5" s="13"/>
       <c r="O5" s="12"/>
     </row>
-    <row r="6" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>1</v>
       </c>
@@ -767,9 +753,7 @@
       <c r="D6" s="13">
         <v>0</v>
       </c>
-      <c r="E6" s="13">
-        <v>0</v>
-      </c>
+      <c r="E6" s="13"/>
       <c r="F6" s="13">
         <v>10</v>
       </c>
@@ -788,16 +772,14 @@
       <c r="K6" s="13">
         <v>0</v>
       </c>
-      <c r="L6" s="13">
-        <v>0</v>
-      </c>
+      <c r="L6" s="13"/>
       <c r="M6" s="13">
         <v>0</v>
       </c>
       <c r="N6" s="12"/>
       <c r="O6" s="12"/>
     </row>
-    <row r="7" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>19</v>
       </c>
@@ -810,9 +792,7 @@
       <c r="D7" s="13">
         <v>0</v>
       </c>
-      <c r="E7" s="13">
-        <v>0</v>
-      </c>
+      <c r="E7" s="13"/>
       <c r="F7" s="13">
         <v>0</v>
       </c>
@@ -831,16 +811,14 @@
       <c r="K7" s="13">
         <v>0</v>
       </c>
-      <c r="L7" s="13">
-        <v>0</v>
-      </c>
+      <c r="L7" s="13"/>
       <c r="M7" s="13">
         <v>0</v>
       </c>
       <c r="N7" s="13"/>
       <c r="O7" s="12"/>
     </row>
-    <row r="8" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>2</v>
       </c>
@@ -853,9 +831,7 @@
       <c r="D8" s="13">
         <v>0</v>
       </c>
-      <c r="E8" s="13">
-        <v>0</v>
-      </c>
+      <c r="E8" s="13"/>
       <c r="F8" s="13">
         <v>0</v>
       </c>
@@ -874,16 +850,14 @@
       <c r="K8" s="13">
         <v>0</v>
       </c>
-      <c r="L8" s="13">
-        <v>0</v>
-      </c>
+      <c r="L8" s="13"/>
       <c r="M8" s="13">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="N8" s="12"/>
       <c r="O8" s="13"/>
     </row>
-    <row r="9" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>3</v>
       </c>
@@ -896,11 +870,9 @@
       <c r="D9" s="13">
         <v>1</v>
       </c>
-      <c r="E9" s="13">
-        <v>0</v>
-      </c>
+      <c r="E9" s="13"/>
       <c r="F9" s="13">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G9" s="13">
         <v>4</v>
@@ -909,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="I9" s="13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J9" s="13">
         <v>0</v>
@@ -917,16 +889,14 @@
       <c r="K9" s="13">
         <v>0</v>
       </c>
-      <c r="L9" s="13">
-        <v>0</v>
-      </c>
+      <c r="L9" s="13"/>
       <c r="M9" s="13">
         <v>0</v>
       </c>
       <c r="N9" s="12"/>
       <c r="O9" s="13"/>
     </row>
-    <row r="10" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -939,9 +909,7 @@
       <c r="D10" s="12">
         <v>0</v>
       </c>
-      <c r="E10" s="12">
-        <v>0</v>
-      </c>
+      <c r="E10" s="12"/>
       <c r="F10" s="12">
         <v>0</v>
       </c>
@@ -960,16 +928,14 @@
       <c r="K10" s="12">
         <v>0</v>
       </c>
-      <c r="L10" s="12">
-        <v>0</v>
-      </c>
+      <c r="L10" s="12"/>
       <c r="M10" s="12">
         <v>0</v>
       </c>
       <c r="N10" s="12"/>
       <c r="O10" s="12"/>
     </row>
-    <row r="11" spans="1:15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>4</v>
       </c>
@@ -985,13 +951,9 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="E11" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="E11" s="13"/>
       <c r="F11" s="13">
-        <f t="shared" si="0"/>
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
@@ -1003,30 +965,27 @@
       </c>
       <c r="I11" s="13">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J11" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K11" s="13">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="L11" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="L11" s="13"/>
       <c r="M11" s="13">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="N11" s="13"/>
       <c r="O11" s="13"/>
     </row>
-    <row r="13" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B13" s="22"/>
       <c r="C13" s="22"/>
@@ -1038,7 +997,7 @@
       <c r="I13" s="22"/>
       <c r="J13" s="22"/>
     </row>
-    <row r="14" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="22"/>
       <c r="B14" s="22"/>
       <c r="C14" s="22"/>
@@ -1050,7 +1009,7 @@
       <c r="I14" s="22"/>
       <c r="J14" s="22"/>
     </row>
-    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="22"/>
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
@@ -1062,7 +1021,7 @@
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
     </row>
-    <row r="16" spans="1:15" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>5</v>
       </c>
@@ -1079,7 +1038,7 @@
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
     </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19"/>
       <c r="B17" s="19"/>
       <c r="C17" s="19"/>
@@ -1094,7 +1053,7 @@
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
     </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19"/>
       <c r="B18" s="19"/>
       <c r="C18" s="19"/>
@@ -1109,7 +1068,7 @@
       <c r="L18" s="19"/>
       <c r="M18" s="19"/>
     </row>
-    <row r="19" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19"/>
       <c r="B19" s="19"/>
       <c r="C19" s="19"/>
@@ -1124,7 +1083,7 @@
       <c r="L19" s="19"/>
       <c r="M19" s="19"/>
     </row>
-    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -1139,7 +1098,7 @@
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
     </row>
-    <row r="21" spans="1:13" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="8" t="s">
         <v>6</v>
       </c>
@@ -1162,7 +1121,7 @@
       <c r="L21" s="20"/>
       <c r="M21" s="20"/>
     </row>
-    <row r="22" spans="1:13" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="15.6" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12" t="s">
         <v>22</v>
       </c>
@@ -1181,7 +1140,7 @@
       <c r="L22" s="23"/>
       <c r="M22" s="23"/>
     </row>
-    <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
         <v>23</v>
       </c>
@@ -1200,7 +1159,7 @@
       <c r="L23" s="24"/>
       <c r="M23" s="24"/>
     </row>
-    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
         <v>24</v>
       </c>
@@ -1219,12 +1178,12 @@
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
     </row>
-    <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B25" s="2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="26"/>
@@ -1238,9 +1197,9 @@
       <c r="L25" s="27"/>
       <c r="M25" s="28"/>
     </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2">
         <v>5</v>
@@ -1257,9 +1216,9 @@
       <c r="L26" s="27"/>
       <c r="M26" s="28"/>
     </row>
-    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2">
         <v>1</v>
@@ -1276,9 +1235,9 @@
       <c r="L27" s="27"/>
       <c r="M27" s="28"/>
     </row>
-    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2">
         <v>2</v>
@@ -1295,9 +1254,9 @@
       <c r="L28" s="27"/>
       <c r="M28" s="28"/>
     </row>
-    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>3</v>
@@ -1314,9 +1273,9 @@
       <c r="L29" s="27"/>
       <c r="M29" s="28"/>
     </row>
-    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>3</v>
@@ -1333,9 +1292,9 @@
       <c r="L30" s="27"/>
       <c r="M30" s="28"/>
     </row>
-    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2">
         <v>8</v>
@@ -1352,13 +1311,9 @@
       <c r="L31" s="16"/>
       <c r="M31" s="16"/>
     </row>
-    <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="B32" s="2">
-        <v>2</v>
-      </c>
+    <row r="32" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="15"/>
+      <c r="B32" s="2"/>
       <c r="C32" s="14"/>
       <c r="D32" s="16"/>
       <c r="E32" s="16"/>
@@ -1371,7 +1326,7 @@
       <c r="L32" s="16"/>
       <c r="M32" s="16"/>
     </row>
-    <row r="33" spans="1:13" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A33" s="10"/>
       <c r="B33" s="2"/>
       <c r="C33" s="14"/>
@@ -1386,10 +1341,10 @@
       <c r="L33" s="17"/>
       <c r="M33" s="17"/>
     </row>
-    <row r="34" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="35" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:13" ht="12.75" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:13" ht="13.2" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
@@ -1397,7 +1352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
         <v>17</v>
       </c>
@@ -1405,7 +1360,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
         <v>16</v>
       </c>
@@ -1413,7 +1368,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
         <v>15</v>
       </c>
@@ -1421,7 +1376,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
complete sprint 8 data
</commit_message>
<xml_diff>
--- a/feebacks-timesheets/Sprint8_Timesheet.xlsx
+++ b/feebacks-timesheets/Sprint8_Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asarpa\Desktop\thesis\feebacks-timesheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87F09C60-F08B-4414-B521-888DF2C9331E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BAA1928-EC4C-4178-AF1D-E989F8AF49AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="36">
   <si>
     <t>Amedeo</t>
   </si>
@@ -130,6 +130,15 @@
   </si>
   <si>
     <t>charly 11/07</t>
+  </si>
+  <si>
+    <t>not finished</t>
+  </si>
+  <si>
+    <t>underestimated; we add two pie charts, and was not planned</t>
+  </si>
+  <si>
+    <t>underestimated; we forgot stuff during the planning</t>
   </si>
 </sst>
 </file>
@@ -596,8 +605,8 @@
   </sheetPr>
   <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -722,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="13">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I5" s="13">
         <v>0</v>
@@ -731,7 +740,7 @@
         <v>7</v>
       </c>
       <c r="K5" s="13">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L5" s="13"/>
       <c r="M5" s="13">
@@ -767,7 +776,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="13">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K6" s="13">
         <v>0</v>
@@ -948,7 +957,7 @@
         <v>1</v>
       </c>
       <c r="D11" s="13">
-        <f t="shared" si="0"/>
+        <f>SUM(D5:D10)</f>
         <v>1</v>
       </c>
       <c r="E11" s="13"/>
@@ -956,12 +965,12 @@
         <v>31</v>
       </c>
       <c r="G11" s="13">
-        <f t="shared" si="0"/>
+        <f>SUM(G5:G10)</f>
         <v>4</v>
       </c>
       <c r="H11" s="13">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I11" s="13">
         <f t="shared" si="0"/>
@@ -969,11 +978,11 @@
       </c>
       <c r="J11" s="13">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="K11" s="13">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="L11" s="13"/>
       <c r="M11" s="13">
@@ -1204,7 +1213,9 @@
       <c r="B26" s="2">
         <v>5</v>
       </c>
-      <c r="C26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D26" s="26"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
@@ -1259,9 +1270,11 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>3</v>
-      </c>
-      <c r="C29" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="D29" s="26"/>
       <c r="E29" s="27"/>
       <c r="F29" s="27"/>
@@ -1296,8 +1309,8 @@
       <c r="A31" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="2">
-        <v>8</v>
+      <c r="B31" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="16"/>

</xml_diff>